<commit_message>
These are the terrible outputs from changing FL to 0.01-0.5, make sure to change the .m and xlsx files back using git checkout
</commit_message>
<xml_diff>
--- a/AIC9parameters_FinalConfirmation_moredata.xlsx
+++ b/AIC9parameters_FinalConfirmation_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FE95ED-9E55-4968-84F6-3395A6920165}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D426AF-6F99-47CA-A6EE-96D5CAC5CED9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="2835" windowWidth="17280" windowHeight="9030" xr2:uid="{DAE4A6D3-542D-42F9-A3B6-815A2B125BD5}"/>
+    <workbookView xWindow="3180" yWindow="3180" windowWidth="17280" windowHeight="9030" xr2:uid="{DAE4A6D3-542D-42F9-A3B6-815A2B125BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,10 +390,10 @@
         <v>2204.2292170912619</v>
       </c>
       <c r="B1">
-        <v>1383.0965219650079</v>
+        <v>1383.0965220845178</v>
       </c>
       <c r="C1">
-        <v>1428.823605990543</v>
+        <v>1428.823605919041</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -401,230 +401,230 @@
         <v>2227.1192368922416</v>
       </c>
       <c r="B2">
-        <v>1482.0442398488944</v>
+        <v>1482.0442259078409</v>
       </c>
       <c r="C2">
-        <v>1329.6420023845887</v>
+        <v>1329.6420705791181</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2343.9137069531039</v>
+        <v>2343.9137069531043</v>
       </c>
       <c r="B3">
-        <v>1585.8750567376301</v>
+        <v>1585.8755819885312</v>
       </c>
       <c r="C3">
-        <v>1454.0892310244092</v>
+        <v>1454.0869954572026</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2320.9625073864663</v>
+        <v>2320.9625000851147</v>
       </c>
       <c r="B4">
-        <v>1788.7195930546336</v>
+        <v>1780.0461948646082</v>
       </c>
       <c r="C4">
-        <v>1763.2947254090432</v>
+        <v>1731.5928878222501</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2422.6539933955587</v>
+        <v>2422.6595198945024</v>
       </c>
       <c r="B5">
-        <v>1669.0272781903411</v>
+        <v>1674.9654899696432</v>
       </c>
       <c r="C5">
-        <v>1624.4305377220869</v>
+        <v>1622.5281738093465</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2360.7084402309279</v>
+        <v>2360.7084402304272</v>
       </c>
       <c r="B6">
-        <v>1774.6285770614304</v>
+        <v>1774.6285757658027</v>
       </c>
       <c r="C6">
-        <v>1784.432976973259</v>
+        <v>1784.4329783711232</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1992.9848472507151</v>
+        <v>1992.9848472506942</v>
       </c>
       <c r="B7">
-        <v>1566.2947814339752</v>
+        <v>1566.2947458768306</v>
       </c>
       <c r="C7">
-        <v>1482.2945271321751</v>
+        <v>1482.2946237954445</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2135.6723079001295</v>
+        <v>2135.7478628450635</v>
       </c>
       <c r="B8">
-        <v>1612.0574530051363</v>
+        <v>1655.7390016109439</v>
       </c>
       <c r="C8">
-        <v>1679.2576002754586</v>
+        <v>1507.3584903465025</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2471.0153725349251</v>
+        <v>2471.0184236373766</v>
       </c>
       <c r="B9">
-        <v>1788.3095594075089</v>
+        <v>1806.1208547647914</v>
       </c>
       <c r="C9">
-        <v>1513.8952422040152</v>
+        <v>1570.5840636497583</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2111.5947501270725</v>
+        <v>2111.5944043737513</v>
       </c>
       <c r="B10">
-        <v>1359.5436219266949</v>
+        <v>1384.8197897029249</v>
       </c>
       <c r="C10">
-        <v>1316.8044372235104</v>
+        <v>1313.1822179032408</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1970.003883917462</v>
+        <v>1970.0049584060432</v>
       </c>
       <c r="B11">
-        <v>1416.252990930532</v>
+        <v>1414.6269501252143</v>
       </c>
       <c r="C11">
-        <v>1298.4013269022387</v>
+        <v>1312.1828705205139</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2787.953718940531</v>
+        <v>2787.9537156936608</v>
       </c>
       <c r="B12">
-        <v>2270.4393957721932</v>
+        <v>2270.4398262776958</v>
       </c>
       <c r="C12">
-        <v>2036.7347968306058</v>
+        <v>2036.7362819098314</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2315.1853419622416</v>
+        <v>2315.1858317581732</v>
       </c>
       <c r="B13">
-        <v>1782.1432978595883</v>
+        <v>1777.4423331486139</v>
       </c>
       <c r="C13">
-        <v>1792.043876782089</v>
+        <v>1794.9018703913953</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2593.0484713468654</v>
+        <v>2593.0482642470733</v>
       </c>
       <c r="B14">
-        <v>1922.7160414204643</v>
+        <v>1924.4781793533441</v>
       </c>
       <c r="C14">
-        <v>1702.3625413241564</v>
+        <v>1698.5718122336648</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2508.3188497746851</v>
+        <v>2508.5108803272624</v>
       </c>
       <c r="B15">
-        <v>2002.6740676254963</v>
+        <v>2026.7228967099065</v>
       </c>
       <c r="C15">
-        <v>2042.0927244971056</v>
+        <v>1827.5083266369336</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2205.5211166450963</v>
+        <v>2205.5211166519052</v>
       </c>
       <c r="B16">
-        <v>1510.1431157823199</v>
+        <v>1546.5982352544029</v>
       </c>
       <c r="C16">
-        <v>1270.5712433044525</v>
+        <v>1276.461477199553</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2225.5452594753074</v>
+        <v>2225.5448130781733</v>
       </c>
       <c r="B17">
-        <v>1686.5873845206668</v>
+        <v>1682.2603177883561</v>
       </c>
       <c r="C17">
-        <v>1564.3984569351537</v>
+        <v>1573.6650186867739</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2487.9072684430239</v>
+        <v>2487.9072724582679</v>
       </c>
       <c r="B18">
-        <v>2061.2592440794292</v>
+        <v>2063.1343444789436</v>
       </c>
       <c r="C18">
-        <v>1916.9784886481884</v>
+        <v>1909.7693489385661</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1742.2116480415741</v>
+        <v>1761.81626294991</v>
       </c>
       <c r="B19">
-        <v>1927.5181621920403</v>
+        <v>1928.7684870713738</v>
       </c>
       <c r="C19">
-        <v>1884.7058218307263</v>
+        <v>1884.2930518248493</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2351.256836519733</v>
+        <v>2351.2568365245052</v>
       </c>
       <c r="B20">
-        <v>1850.0736740607986</v>
+        <v>1850.0736691983486</v>
       </c>
       <c r="C20">
-        <v>1653.3462287517611</v>
+        <v>1653.3462609483511</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2583.1100843896215</v>
+        <v>2583.1100843929667</v>
       </c>
       <c r="B21">
-        <v>1907.0148737384604</v>
+        <v>1907.0148615932583</v>
       </c>
       <c r="C21">
-        <v>1813.0877816457973</v>
+        <v>1813.087800925716</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2448.3691808016056</v>
+        <v>2448.3691807967398</v>
       </c>
       <c r="B22">
-        <v>1890.2457143793833</v>
+        <v>1890.2457180811034</v>
       </c>
       <c r="C22">
-        <v>1644.281117503079</v>
+        <v>1644.2810920719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
These are the bad results from running FL from 0.1-0.8
</commit_message>
<xml_diff>
--- a/AIC9parameters_FinalConfirmation_moredata.xlsx
+++ b/AIC9parameters_FinalConfirmation_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D426AF-6F99-47CA-A6EE-96D5CAC5CED9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1B0D79-E45F-41CC-B656-DC5998C3F48E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="3180" windowWidth="17280" windowHeight="9030" xr2:uid="{DAE4A6D3-542D-42F9-A3B6-815A2B125BD5}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{DAE4A6D3-542D-42F9-A3B6-815A2B125BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,244 +387,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2204.2292170912619</v>
+        <v>2204.2292171065692</v>
       </c>
       <c r="B1">
-        <v>1383.0965220845178</v>
+        <v>1384.9784196034625</v>
       </c>
       <c r="C1">
-        <v>1428.823605919041</v>
+        <v>1432.3647031410342</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2227.1192368922416</v>
+        <v>2227.1217362298958</v>
       </c>
       <c r="B2">
-        <v>1482.0442259078409</v>
+        <v>1437.8378068311729</v>
       </c>
       <c r="C2">
-        <v>1329.6420705791181</v>
+        <v>1597.6623857966588</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2343.9137069531043</v>
+        <v>2343.9137069389285</v>
       </c>
       <c r="B3">
-        <v>1585.8755819885312</v>
+        <v>1562.5519803917387</v>
       </c>
       <c r="C3">
-        <v>1454.0869954572026</v>
+        <v>1546.0202461918882</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2320.9625000851147</v>
+        <v>2320.9625107300044</v>
       </c>
       <c r="B4">
-        <v>1780.0461948646082</v>
+        <v>1777.2019743706417</v>
       </c>
       <c r="C4">
-        <v>1731.5928878222501</v>
+        <v>1719.7151079426428</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2422.6595198945024</v>
+        <v>2422.6539933914073</v>
       </c>
       <c r="B5">
-        <v>1674.9654899696432</v>
+        <v>1667.3574578925873</v>
       </c>
       <c r="C5">
-        <v>1622.5281738093465</v>
+        <v>1629.5498009388937</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2360.7084402304272</v>
+        <v>2360.708401255838</v>
       </c>
       <c r="B6">
-        <v>1774.6285757658027</v>
+        <v>1774.6928232753951</v>
       </c>
       <c r="C6">
-        <v>1784.4329783711232</v>
+        <v>1784.4776913416292</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1992.9848472506942</v>
+        <v>1992.9848978898274</v>
       </c>
       <c r="B7">
-        <v>1566.2947458768306</v>
+        <v>1566.2710828612082</v>
       </c>
       <c r="C7">
-        <v>1482.2946237954445</v>
+        <v>1484.2211590598711</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2135.7478628450635</v>
+        <v>2135.7478628526442</v>
       </c>
       <c r="B8">
-        <v>1655.7390016109439</v>
+        <v>1655.7390018863714</v>
       </c>
       <c r="C8">
-        <v>1507.3584903465025</v>
+        <v>1507.3584775010195</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2471.0184236373766</v>
+        <v>2471.0177526676862</v>
       </c>
       <c r="B9">
-        <v>1806.1208547647914</v>
+        <v>1800.6029858790894</v>
       </c>
       <c r="C9">
-        <v>1570.5840636497583</v>
+        <v>1551.7456437379697</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2111.5944043737513</v>
+        <v>2111.6060965539632</v>
       </c>
       <c r="B10">
-        <v>1384.8197897029249</v>
+        <v>1384.7449821684261</v>
       </c>
       <c r="C10">
-        <v>1313.1822179032408</v>
+        <v>1362.2270035448807</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1970.0049584060432</v>
+        <v>1970.0038839174615</v>
       </c>
       <c r="B11">
-        <v>1414.6269501252143</v>
+        <v>1416.2529893939627</v>
       </c>
       <c r="C11">
-        <v>1312.1828705205139</v>
+        <v>1298.4013325128637</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2787.9537156936608</v>
+        <v>2787.9537061107872</v>
       </c>
       <c r="B12">
-        <v>2270.4398262776958</v>
+        <v>2270.4411671699713</v>
       </c>
       <c r="C12">
-        <v>2036.7362819098314</v>
+        <v>2036.7399429835384</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2315.1858317581732</v>
+        <v>2315.185341097801</v>
       </c>
       <c r="B13">
-        <v>1777.4423331486139</v>
+        <v>1763.908795922524</v>
       </c>
       <c r="C13">
-        <v>1794.9018703913953</v>
+        <v>1803.6381877513845</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2593.0482642470733</v>
+        <v>2593.0481325924952</v>
       </c>
       <c r="B14">
-        <v>1924.4781793533441</v>
+        <v>1919.8514062571228</v>
       </c>
       <c r="C14">
-        <v>1698.5718122336648</v>
+        <v>1771.5022962243368</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2508.5108803272624</v>
+        <v>2508.3211273020761</v>
       </c>
       <c r="B15">
-        <v>2026.7228967099065</v>
+        <v>2032.9295184874288</v>
       </c>
       <c r="C15">
-        <v>1827.5083266369336</v>
+        <v>1966.7636030502799</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2205.5211166519052</v>
+        <v>2205.5211166496383</v>
       </c>
       <c r="B16">
-        <v>1546.5982352544029</v>
+        <v>1536.4424786824784</v>
       </c>
       <c r="C16">
-        <v>1276.461477199553</v>
+        <v>1270.3318538283795</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2225.5448130781733</v>
+        <v>2225.5448111673422</v>
       </c>
       <c r="B17">
-        <v>1682.2603177883561</v>
+        <v>1678.4907154266741</v>
       </c>
       <c r="C17">
-        <v>1573.6650186867739</v>
+        <v>1588.4518536184632</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2487.9072724582679</v>
+        <v>2487.9072684430193</v>
       </c>
       <c r="B18">
-        <v>2063.1343444789436</v>
+        <v>2061.2592403222206</v>
       </c>
       <c r="C18">
-        <v>1909.7693489385661</v>
+        <v>1916.9785060868273</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1761.81626294991</v>
+        <v>1810.972624286753</v>
       </c>
       <c r="B19">
-        <v>1928.7684870713738</v>
+        <v>1940.946478028055</v>
       </c>
       <c r="C19">
-        <v>1884.2930518248493</v>
+        <v>1955.4582997565253</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2351.2568365245052</v>
+        <v>2351.2568365264019</v>
       </c>
       <c r="B20">
-        <v>1850.0736691983486</v>
+        <v>1850.0736672655316</v>
       </c>
       <c r="C20">
-        <v>1653.3462609483511</v>
+        <v>1653.3462737461939</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2583.1100843929667</v>
+        <v>2583.110078207194</v>
       </c>
       <c r="B21">
-        <v>1907.0148615932583</v>
+        <v>1907.0371173723911</v>
       </c>
       <c r="C21">
-        <v>1813.087800925716</v>
+        <v>1813.052769841026</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2448.3691807967398</v>
+        <v>2448.3691807930336</v>
       </c>
       <c r="B22">
-        <v>1890.2457180811034</v>
+        <v>1890.2457209890522</v>
       </c>
       <c r="C22">
-        <v>1644.2810920719</v>
+        <v>1644.281071491549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
These are slightly worse results after changing initial condition to 0.1
</commit_message>
<xml_diff>
--- a/AIC9parameters_FinalConfirmation_moredata.xlsx
+++ b/AIC9parameters_FinalConfirmation_moredata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1B0D79-E45F-41CC-B656-DC5998C3F48E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958ADB6D-EC26-4B3A-9685-DF08B5A418C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{DAE4A6D3-542D-42F9-A3B6-815A2B125BD5}"/>
   </bookViews>
@@ -387,244 +387,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2204.2292171065692</v>
+        <v>2204.2292171047425</v>
       </c>
       <c r="B1">
-        <v>1384.9784196034625</v>
+        <v>1384.3421185015861</v>
       </c>
       <c r="C1">
-        <v>1432.3647031410342</v>
+        <v>1431.1789760132535</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2227.1217362298958</v>
+        <v>2227.1192368922416</v>
       </c>
       <c r="B2">
-        <v>1437.8378068311729</v>
+        <v>1482.0442411429403</v>
       </c>
       <c r="C2">
-        <v>1597.6623857966588</v>
+        <v>1329.6419960545563</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2343.9137069389285</v>
+        <v>2343.913706953103</v>
       </c>
       <c r="B3">
-        <v>1562.5519803917387</v>
+        <v>1585.8742932348805</v>
       </c>
       <c r="C3">
-        <v>1546.0202461918882</v>
+        <v>1454.0924806953633</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2320.9625107300044</v>
+        <v>2320.9625221260826</v>
       </c>
       <c r="B4">
-        <v>1777.2019743706417</v>
+        <v>1774.3335864583587</v>
       </c>
       <c r="C4">
-        <v>1719.7151079426428</v>
+        <v>1704.2599074406442</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2422.6539933914073</v>
+        <v>2422.6539934395523</v>
       </c>
       <c r="B5">
-        <v>1667.3574578925873</v>
+        <v>1668.399809907037</v>
       </c>
       <c r="C5">
-        <v>1629.5498009388937</v>
+        <v>1626.0505420097888</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2360.708401255838</v>
+        <v>2360.7084017193019</v>
       </c>
       <c r="B6">
-        <v>1774.6928232753951</v>
+        <v>1774.9878092462952</v>
       </c>
       <c r="C6">
-        <v>1784.4776913416292</v>
+        <v>1784.9998764703353</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1992.9848978898274</v>
+        <v>1992.9848472506753</v>
       </c>
       <c r="B7">
-        <v>1566.2710828612082</v>
+        <v>1566.2947138691036</v>
       </c>
       <c r="C7">
-        <v>1484.2211590598711</v>
+        <v>1482.2947108097806</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2135.7478628526442</v>
+        <v>2135.7478628374106</v>
       </c>
       <c r="B8">
-        <v>1655.7390018863714</v>
+        <v>1655.7390014213242</v>
       </c>
       <c r="C8">
-        <v>1507.3584775010195</v>
+        <v>1507.3585028172008</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2471.0177526676862</v>
+        <v>2471.0153725333803</v>
       </c>
       <c r="B9">
-        <v>1800.6029858790894</v>
+        <v>1788.3101470495083</v>
       </c>
       <c r="C9">
-        <v>1551.7456437379697</v>
+        <v>1513.896066139911</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2111.6060965539632</v>
+        <v>2111.5944042664491</v>
       </c>
       <c r="B10">
-        <v>1384.7449821684261</v>
+        <v>1365.1595641833082</v>
       </c>
       <c r="C10">
-        <v>1362.2270035448807</v>
+        <v>1300.9352233413354</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1970.0038839174615</v>
+        <v>1970.003883917462</v>
       </c>
       <c r="B11">
-        <v>1416.2529893939627</v>
+        <v>1416.2529907667447</v>
       </c>
       <c r="C11">
-        <v>1298.4013325128637</v>
+        <v>1298.4013275002937</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2787.9537061107872</v>
+        <v>2787.95371453083</v>
       </c>
       <c r="B12">
-        <v>2270.4411671699713</v>
+        <v>2270.4399898165884</v>
       </c>
       <c r="C12">
-        <v>2036.7399429835384</v>
+        <v>2036.7367177336491</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2315.185341097801</v>
+        <v>2315.1853419620352</v>
       </c>
       <c r="B13">
-        <v>1763.908795922524</v>
+        <v>1782.3539396052565</v>
       </c>
       <c r="C13">
-        <v>1803.6381877513845</v>
+        <v>1791.9062670150788</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2593.0481325924952</v>
+        <v>2593.0481324833722</v>
       </c>
       <c r="B14">
-        <v>1919.8514062571228</v>
+        <v>1922.4491827528125</v>
       </c>
       <c r="C14">
-        <v>1771.5022962243368</v>
+        <v>1703.8048925083233</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2508.3211273020761</v>
+        <v>2508.5108803790531</v>
       </c>
       <c r="B15">
-        <v>2032.9295184874288</v>
+        <v>2026.7228915761436</v>
       </c>
       <c r="C15">
-        <v>1966.7636030502799</v>
+        <v>1827.5083118642979</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2205.5211166496383</v>
+        <v>2205.521116644954</v>
       </c>
       <c r="B16">
-        <v>1536.4424786824784</v>
+        <v>1510.1697609818998</v>
       </c>
       <c r="C16">
-        <v>1270.3318538283795</v>
+        <v>1270.5287368582376</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2225.5448111673422</v>
+        <v>2225.5448130781629</v>
       </c>
       <c r="B17">
-        <v>1678.4907154266741</v>
+        <v>1682.2602014089707</v>
       </c>
       <c r="C17">
-        <v>1588.4518536184632</v>
+        <v>1573.665397592627</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2487.9072684430193</v>
+        <v>2487.9072684430248</v>
       </c>
       <c r="B18">
-        <v>2061.2592403222206</v>
+        <v>2061.2592446629073</v>
       </c>
       <c r="C18">
-        <v>1916.9785060868273</v>
+        <v>1916.9784859400013</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1810.972624286753</v>
+        <v>1742.2116489556101</v>
       </c>
       <c r="B19">
-        <v>1940.946478028055</v>
+        <v>1927.5181691925923</v>
       </c>
       <c r="C19">
-        <v>1955.4582997565253</v>
+        <v>1884.7058103212241</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2351.2568365264019</v>
+        <v>2351.2568365319244</v>
       </c>
       <c r="B20">
-        <v>1850.0736672655316</v>
+        <v>1850.0736616385993</v>
       </c>
       <c r="C20">
-        <v>1653.3462737461939</v>
+        <v>1653.3463110047869</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2583.110078207194</v>
+        <v>2583.1100797798213</v>
       </c>
       <c r="B21">
-        <v>1907.0371173723911</v>
+        <v>1907.0314517922743</v>
       </c>
       <c r="C21">
-        <v>1813.052769841026</v>
+        <v>1813.0616860349023</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2448.3691807930336</v>
+        <v>2448.3691808101894</v>
       </c>
       <c r="B22">
-        <v>1890.2457209890522</v>
+        <v>1890.2457075819934</v>
       </c>
       <c r="C22">
-        <v>1644.281071491549</v>
+        <v>1644.281166023012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made plots for manuscript
</commit_message>
<xml_diff>
--- a/AIC9parameters_FinalConfirmation_moredata.xlsx
+++ b/AIC9parameters_FinalConfirmation_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958ADB6D-EC26-4B3A-9685-DF08B5A418C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A24FDBC-5E57-4C92-88B7-195384CE66A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{DAE4A6D3-542D-42F9-A3B6-815A2B125BD5}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{DAE4A6D3-542D-42F9-A3B6-815A2B125BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,13 +387,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2204.2292171047425</v>
+        <v>2204.2292170912619</v>
       </c>
       <c r="B1">
-        <v>1384.3421185015861</v>
+        <v>1383.0965219650079</v>
       </c>
       <c r="C1">
-        <v>1431.1789760132535</v>
+        <v>1428.823605990543</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -401,98 +401,98 @@
         <v>2227.1192368922416</v>
       </c>
       <c r="B2">
-        <v>1482.0442411429403</v>
+        <v>1482.0442398488944</v>
       </c>
       <c r="C2">
-        <v>1329.6419960545563</v>
+        <v>1329.6420023845887</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2343.913706953103</v>
+        <v>2343.9137069531039</v>
       </c>
       <c r="B3">
-        <v>1585.8742932348805</v>
+        <v>1585.8750567376301</v>
       </c>
       <c r="C3">
-        <v>1454.0924806953633</v>
+        <v>1454.0892310244092</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2320.9625221260826</v>
+        <v>2320.9625073864663</v>
       </c>
       <c r="B4">
-        <v>1774.3335864583587</v>
+        <v>1788.7195930546336</v>
       </c>
       <c r="C4">
-        <v>1704.2599074406442</v>
+        <v>1763.2947254090432</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2422.6539934395523</v>
+        <v>2422.6539933955587</v>
       </c>
       <c r="B5">
-        <v>1668.399809907037</v>
+        <v>1669.0272781903411</v>
       </c>
       <c r="C5">
-        <v>1626.0505420097888</v>
+        <v>1624.4305377220869</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2360.7084017193019</v>
+        <v>2360.7084402309279</v>
       </c>
       <c r="B6">
-        <v>1774.9878092462952</v>
+        <v>1774.6285770614304</v>
       </c>
       <c r="C6">
-        <v>1784.9998764703353</v>
+        <v>1784.432976973259</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1992.9848472506753</v>
+        <v>1992.9848472507151</v>
       </c>
       <c r="B7">
-        <v>1566.2947138691036</v>
+        <v>1566.2947814339752</v>
       </c>
       <c r="C7">
-        <v>1482.2947108097806</v>
+        <v>1482.2945271321751</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2135.7478628374106</v>
+        <v>2135.6723079001295</v>
       </c>
       <c r="B8">
-        <v>1655.7390014213242</v>
+        <v>1612.0574530051363</v>
       </c>
       <c r="C8">
-        <v>1507.3585028172008</v>
+        <v>1679.2576002754586</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2471.0153725333803</v>
+        <v>2471.0153725349251</v>
       </c>
       <c r="B9">
-        <v>1788.3101470495083</v>
+        <v>1788.3095594075089</v>
       </c>
       <c r="C9">
-        <v>1513.896066139911</v>
+        <v>1513.8952422040152</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2111.5944042664491</v>
+        <v>2111.5947501270725</v>
       </c>
       <c r="B10">
-        <v>1365.1595641833082</v>
+        <v>1359.5436219266949</v>
       </c>
       <c r="C10">
-        <v>1300.9352233413354</v>
+        <v>1316.8044372235104</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -500,131 +500,131 @@
         <v>1970.003883917462</v>
       </c>
       <c r="B11">
-        <v>1416.2529907667447</v>
+        <v>1416.252990930532</v>
       </c>
       <c r="C11">
-        <v>1298.4013275002937</v>
+        <v>1298.4013269022387</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2787.95371453083</v>
+        <v>2787.953718940531</v>
       </c>
       <c r="B12">
-        <v>2270.4399898165884</v>
+        <v>2270.4393957721932</v>
       </c>
       <c r="C12">
-        <v>2036.7367177336491</v>
+        <v>2036.7347968306058</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2315.1853419620352</v>
+        <v>2315.1853419622416</v>
       </c>
       <c r="B13">
-        <v>1782.3539396052565</v>
+        <v>1782.1432978595883</v>
       </c>
       <c r="C13">
-        <v>1791.9062670150788</v>
+        <v>1792.043876782089</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2593.0481324833722</v>
+        <v>2593.0484713468654</v>
       </c>
       <c r="B14">
-        <v>1922.4491827528125</v>
+        <v>1922.7160414204643</v>
       </c>
       <c r="C14">
-        <v>1703.8048925083233</v>
+        <v>1702.3625413241564</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2508.5108803790531</v>
+        <v>2508.3188497746851</v>
       </c>
       <c r="B15">
-        <v>2026.7228915761436</v>
+        <v>2002.6740676254963</v>
       </c>
       <c r="C15">
-        <v>1827.5083118642979</v>
+        <v>2042.0927244971056</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2205.521116644954</v>
+        <v>2205.5211166450963</v>
       </c>
       <c r="B16">
-        <v>1510.1697609818998</v>
+        <v>1510.1431157823199</v>
       </c>
       <c r="C16">
-        <v>1270.5287368582376</v>
+        <v>1270.5712433044525</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2225.5448130781629</v>
+        <v>2225.5452594753074</v>
       </c>
       <c r="B17">
-        <v>1682.2602014089707</v>
+        <v>1686.5873845206668</v>
       </c>
       <c r="C17">
-        <v>1573.665397592627</v>
+        <v>1564.3984569351537</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2487.9072684430248</v>
+        <v>2487.9072684430239</v>
       </c>
       <c r="B18">
-        <v>2061.2592446629073</v>
+        <v>2061.2592440794292</v>
       </c>
       <c r="C18">
-        <v>1916.9784859400013</v>
+        <v>1916.9784886481884</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1742.2116489556101</v>
+        <v>1742.2116480415741</v>
       </c>
       <c r="B19">
-        <v>1927.5181691925923</v>
+        <v>1927.5181621920403</v>
       </c>
       <c r="C19">
-        <v>1884.7058103212241</v>
+        <v>1884.7058218307263</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2351.2568365319244</v>
+        <v>2351.256836519733</v>
       </c>
       <c r="B20">
-        <v>1850.0736616385993</v>
+        <v>1850.0736740607986</v>
       </c>
       <c r="C20">
-        <v>1653.3463110047869</v>
+        <v>1653.3462287517611</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2583.1100797798213</v>
+        <v>2583.1100843896215</v>
       </c>
       <c r="B21">
-        <v>1907.0314517922743</v>
+        <v>1907.0148737384604</v>
       </c>
       <c r="C21">
-        <v>1813.0616860349023</v>
+        <v>1813.0877816457973</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2448.3691808101894</v>
+        <v>2448.3691808016056</v>
       </c>
       <c r="B22">
-        <v>1890.2457075819934</v>
+        <v>1890.2457143793833</v>
       </c>
       <c r="C22">
-        <v>1644.281166023012</v>
+        <v>1644.281117503079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>